<commit_message>
Typo fix in Livrables
</commit_message>
<xml_diff>
--- a/.informations/Livrables/Guillaume Le Blanc/Livrable2-Scénario.xlsx
+++ b/.informations/Livrables/Guillaume Le Blanc/Livrable2-Scénario.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hymperia\.informations\ScénarioUtilisation\Guillaume Le Blanc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1457093\hymperia\.informations\Livrables\Guillaume Le Blanc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -659,7 +659,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,12 +725,12 @@
         <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>46</v>

</xml_diff>